<commit_message>
Modified the excel sheet with sheets for neuron threshold detection experiment
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucsdcloud-my.sharepoint.com/personal/s3jain_ucsd_edu/Documents/research/IFAT6/Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1425" documentId="11_F25DC773A252ABDACC10481A61DB4E085BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D23862AD-720D-4C37-AE73-08F1D8753012}"/>
+  <xr:revisionPtr revIDLastSave="1456" documentId="11_F25DC773A252ABDACC10481A61DB4E085BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A19914DA-C451-4F4A-BEF1-27E48F912F96}"/>
   <bookViews>
-    <workbookView xWindow="19635" yWindow="0" windowWidth="18915" windowHeight="21705" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="218" yWindow="0" windowWidth="21585" windowHeight="14385" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Core 0" sheetId="1" r:id="rId1"/>
@@ -227,8 +227,8 @@
       <xdr:rowOff>137948</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3279424" cy="1099788"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -270,6 +270,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -504,6 +505,7 @@
               </a:endParaRPr>
             </a:p>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -527,7 +529,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -540,7 +542,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -554,7 +556,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -569,7 +571,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -582,7 +584,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -596,7 +598,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -610,7 +612,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -624,7 +626,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -637,7 +639,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -651,7 +653,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -663,7 +665,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -679,7 +681,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -693,7 +695,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -706,7 +708,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -720,7 +722,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -748,7 +750,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -762,7 +764,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -775,7 +777,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -789,7 +791,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -803,7 +805,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -817,7 +819,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -830,7 +832,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -842,7 +844,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -866,7 +868,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -878,7 +880,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -894,6 +896,7 @@
               </a:endParaRPr>
             </a:p>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -906,7 +909,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -920,6 +923,7 @@
               </a:endParaRPr>
             </a:p>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -932,7 +936,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -946,7 +950,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -961,7 +965,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -974,7 +978,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -988,7 +992,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -1002,7 +1006,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -1016,7 +1020,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -1029,7 +1033,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -1043,7 +1047,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -1055,7 +1059,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -1071,7 +1075,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1085,7 +1089,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -1098,7 +1102,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -1112,7 +1116,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -1130,19 +1134,7 @@
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
-                      <m:t>&gt;</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1"/>
-                        </a:solidFill>
-                        <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:rPr>
-                      <m:t>8</m:t>
+                      <m:t>&gt;8</m:t>
                     </m:r>
                     <m:sSub>
                       <m:sSubPr>
@@ -1152,7 +1144,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -1165,7 +1157,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -1179,7 +1171,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -1193,7 +1185,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1207,7 +1199,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -1220,7 +1212,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -1232,7 +1224,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -1256,7 +1248,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -1268,7 +1260,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -1284,6 +1276,7 @@
               </a:endParaRPr>
             </a:p>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1296,7 +1289,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1312,7 +1305,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -1595,6 +1588,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3187,10 +3184,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA32DAD7-3FF6-4057-A34A-81FA348E3B86}">
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3269,536 +3266,584 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9">
         <v>1</v>
       </c>
-      <c r="B10">
+      <c r="C9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
         <v>47</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>61</v>
-      </c>
-      <c r="C11">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="C12">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C13">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C14">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="C15">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19">
         <v>47</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>2</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <v>6</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <v>39</v>
-      </c>
-      <c r="C21">
-        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C22">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C24">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25">
+        <v>63</v>
+      </c>
+      <c r="C25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26">
         <v>12</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>3</v>
       </c>
-      <c r="B27">
+      <c r="B29">
         <v>50</v>
       </c>
-      <c r="C27">
+      <c r="C29">
         <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28">
-        <v>12</v>
-      </c>
-      <c r="C28">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29">
-        <v>23</v>
-      </c>
-      <c r="C29">
-        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="C30">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C31">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C32">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B33">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C33">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C34">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="C35">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="C36">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C37">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38">
+        <v>22</v>
+      </c>
+      <c r="C38">
         <v>12</v>
-      </c>
-      <c r="C38">
-        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C39">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="C40">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41">
+        <v>56</v>
+      </c>
+      <c r="C41">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>63</v>
+      </c>
+      <c r="C42">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43">
         <v>8</v>
       </c>
-      <c r="C41">
+      <c r="C43">
         <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>4</v>
-      </c>
-      <c r="B43">
-        <v>13</v>
-      </c>
-      <c r="C43">
-        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="C44">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>4</v>
+      </c>
+      <c r="B46">
+        <v>13</v>
+      </c>
+      <c r="C46">
         <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45">
-        <v>63</v>
-      </c>
-      <c r="C45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46">
-        <v>63</v>
-      </c>
-      <c r="C46">
-        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="C47">
-        <v>9</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>63</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>5</v>
-      </c>
       <c r="B49">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="C49">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B50">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="C50">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="C51">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B52">
-        <v>42</v>
-      </c>
-      <c r="C52">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>5</v>
+      </c>
       <c r="B53">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C53">
-        <v>8</v>
+        <v>29</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B54">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="C54">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B55">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C55">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B56">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="C56">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B57">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C57">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B58">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C58">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B59">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C59">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B60">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>47</v>
+      </c>
+      <c r="C61">
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>6</v>
-      </c>
       <c r="B62">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C62">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B63">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="C63">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B64">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="C64">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B65">
-        <v>12</v>
-      </c>
-      <c r="C65">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>6</v>
+      </c>
       <c r="B66">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C66">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B67">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C67">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B68">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="C68">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>12</v>
+      </c>
+      <c r="C69">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>33</v>
+      </c>
+      <c r="C70">
         <v>8</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>7</v>
-      </c>
-      <c r="B70">
-        <v>43</v>
-      </c>
-      <c r="C70">
-        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B71">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C71">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B72">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="C72">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B73">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="C73">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B74">
-        <v>47</v>
-      </c>
-      <c r="C74">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>7</v>
+      </c>
       <c r="B75">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C75">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B76">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="C76">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B77">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C77">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B78">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C78">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B79">
+        <v>47</v>
+      </c>
+      <c r="C79">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>54</v>
+      </c>
+      <c r="C80">
         <v>8</v>
       </c>
-      <c r="C79">
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>50</v>
+      </c>
+      <c r="C81">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>11</v>
+      </c>
+      <c r="C82">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>61</v>
+      </c>
+      <c r="C83">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>8</v>
+      </c>
+      <c r="C84">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>0</v>
+      </c>
+      <c r="C85">
         <v>8</v>
       </c>
     </row>
@@ -3812,8 +3857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EEB2E01-2C42-4EA5-990F-733A63308EA9}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="F1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3922,7 +3967,7 @@
         <v>0.64300000000000002</v>
       </c>
       <c r="H9" s="4">
-        <v>0.57099999999999995</v>
+        <v>0.57199999999999995</v>
       </c>
       <c r="I9" s="4">
         <v>0.51700000000000002</v>
@@ -3942,43 +3987,43 @@
         <v>17</v>
       </c>
       <c r="C11">
-        <f>B9-C9</f>
+        <f t="shared" ref="C11:L11" si="0">B9-C9</f>
         <v>8.0000000000000071E-2</v>
       </c>
       <c r="D11">
-        <f>C9-D9</f>
+        <f t="shared" si="0"/>
         <v>0.15300000000000002</v>
       </c>
       <c r="E11">
-        <f>D9-E9</f>
+        <f t="shared" si="0"/>
         <v>0.18400000000000005</v>
       </c>
       <c r="F11">
-        <f>E9-F9</f>
+        <f t="shared" si="0"/>
         <v>0.18999999999999995</v>
       </c>
       <c r="G11">
-        <f>F9-G9</f>
+        <f t="shared" si="0"/>
         <v>0.11799999999999999</v>
       </c>
       <c r="H11">
-        <f>G9-H9</f>
-        <v>7.2000000000000064E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.1000000000000063E-2</v>
       </c>
       <c r="I11">
-        <f>H9-I9</f>
-        <v>5.3999999999999937E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.4999999999999938E-2</v>
       </c>
       <c r="J11">
-        <f>I9-J9</f>
+        <f t="shared" si="0"/>
         <v>4.9999999999999989E-2</v>
       </c>
       <c r="K11">
-        <f>J9-K9</f>
+        <f t="shared" si="0"/>
         <v>4.6000000000000041E-2</v>
       </c>
       <c r="L11">
-        <f>K9-L9</f>
+        <f t="shared" si="0"/>
         <v>4.5999999999999985E-2</v>
       </c>
     </row>
@@ -3987,47 +4032,47 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <f>1.8-B1</f>
+        <f t="shared" ref="B13:L13" si="1">1.8-B1</f>
         <v>0.7</v>
       </c>
       <c r="C13">
-        <f>1.8-C1</f>
+        <f t="shared" si="1"/>
         <v>0.65000000000000013</v>
       </c>
       <c r="D13">
-        <f>1.8-D1</f>
+        <f t="shared" si="1"/>
         <v>0.60000000000000009</v>
       </c>
       <c r="E13">
-        <f>1.8-E1</f>
+        <f t="shared" si="1"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="F13">
-        <f>1.8-F1</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="G13">
-        <f>1.8-G1</f>
+        <f t="shared" si="1"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="H13">
-        <f>1.8-H1</f>
+        <f t="shared" si="1"/>
         <v>0.40000000000000013</v>
       </c>
       <c r="I13">
-        <f>1.8-I1</f>
+        <f t="shared" si="1"/>
         <v>0.35000000000000009</v>
       </c>
       <c r="J13">
-        <f>1.8-J1</f>
+        <f t="shared" si="1"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="K13">
-        <f>1.8-K1</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="L13">
-        <f>1.8-L1</f>
+        <f t="shared" si="1"/>
         <v>0.19999999999999996</v>
       </c>
     </row>
@@ -4061,7 +4106,7 @@
       </c>
       <c r="H14">
         <f>H9-B3</f>
-        <v>0.37099999999999994</v>
+        <v>0.37199999999999994</v>
       </c>
       <c r="I14">
         <f>I9-B3</f>
@@ -4085,47 +4130,47 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <f>B14-B13</f>
+        <f t="shared" ref="B15:L15" si="2">B14-B13</f>
         <v>0.46800000000000019</v>
       </c>
       <c r="C15">
-        <f>C14-C13</f>
+        <f t="shared" si="2"/>
         <v>0.43799999999999994</v>
       </c>
       <c r="D15">
-        <f>D14-D13</f>
+        <f t="shared" si="2"/>
         <v>0.33499999999999996</v>
       </c>
       <c r="E15">
-        <f>E14-E13</f>
+        <f t="shared" si="2"/>
         <v>0.20099999999999985</v>
       </c>
       <c r="F15">
-        <f>F14-F13</f>
+        <f t="shared" si="2"/>
         <v>6.0999999999999943E-2</v>
       </c>
       <c r="G15">
-        <f>G14-G13</f>
+        <f t="shared" si="2"/>
         <v>-6.9999999999999507E-3</v>
       </c>
       <c r="H15">
-        <f>H14-H13</f>
-        <v>-2.9000000000000192E-2</v>
+        <f t="shared" si="2"/>
+        <v>-2.8000000000000191E-2</v>
       </c>
       <c r="I15">
-        <f>I14-I13</f>
+        <f t="shared" si="2"/>
         <v>-3.3000000000000085E-2</v>
       </c>
       <c r="J15">
-        <f>J14-J13</f>
+        <f t="shared" si="2"/>
         <v>-3.3000000000000029E-2</v>
       </c>
       <c r="K15">
-        <f>K14-K13</f>
+        <f t="shared" si="2"/>
         <v>-2.9000000000000026E-2</v>
       </c>
       <c r="L15">
-        <f>L14-L13</f>
+        <f t="shared" si="2"/>
         <v>-2.4999999999999967E-2</v>
       </c>
     </row>
@@ -4139,8 +4184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AECD8644-96AE-41F5-8CB9-4C3980E79ED9}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4201,7 +4246,7 @@
         <v>18</v>
       </c>
       <c r="B7" s="4">
-        <v>0.57099999999999995</v>
+        <v>0.57199999999999995</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -4219,11 +4264,23 @@
       <c r="A12">
         <v>0</v>
       </c>
+      <c r="B12">
+        <v>52</v>
+      </c>
+      <c r="C12">
+        <v>27</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
+      <c r="B13">
+        <v>43</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -4234,10 +4291,22 @@
       <c r="A15">
         <v>3</v>
       </c>
+      <c r="B15">
+        <v>19</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
+      </c>
+      <c r="B16">
+        <v>63</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>